<commit_message>
Added functions in excel loading to load parameter or other static data from excel files.
</commit_message>
<xml_diff>
--- a/examples/Wealth-Distribution-ParamFromExcel/params.xlsx
+++ b/examples/Wealth-Distribution-ParamFromExcel/params.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12957\Documents\Developing\Python\melodie\tests\resources\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12957\Documents\Developing\Python\melodie\examples\Wealth-Distribution-ParamFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B390D2-DA69-4606-ADCC-345C63DBE496}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED97083D-1F35-415A-8F00-24A50C2D8850}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="12225" activeTab="3" xr2:uid="{716BFD88-6474-41BF-9DB0-21FEC84685E2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="12225" xr2:uid="{716BFD88-6474-41BF-9DB0-21FEC84685E2}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +67,10 @@
   </si>
   <si>
     <t>account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number_of_run</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -458,24 +462,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAC137C-E36E-4AE0-AD87-46B817F3BF1B}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.75" customWidth="1"/>
     <col min="2" max="2" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,26 +488,29 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -510,26 +518,29 @@
         <v>100</v>
       </c>
       <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
         <v>200</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>100</v>
       </c>
-      <c r="F2" s="2">
-        <v>0.5</v>
-      </c>
       <c r="G2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="2">
         <v>100</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>0.6</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -537,26 +548,29 @@
         <v>100</v>
       </c>
       <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
         <v>200</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>100</v>
       </c>
-      <c r="F3" s="2">
-        <v>0.5</v>
-      </c>
       <c r="G3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="2">
         <v>100</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>0.7</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -564,26 +578,29 @@
         <v>100</v>
       </c>
       <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
         <v>200</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>100</v>
       </c>
-      <c r="F4" s="3">
-        <v>0.5</v>
-      </c>
       <c r="G4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="3">
         <v>100</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>0.8</v>
       </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -593,8 +610,9 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -604,8 +622,9 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -615,8 +634,9 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -626,10 +646,12 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2899,7 +2921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AFA9A3E-C4B1-4F8D-873B-B8BE9B181913}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>

</xml_diff>